<commit_message>
Update Account management Test Cases.xlsx
</commit_message>
<xml_diff>
--- a/Common Documents/Test Cases/Account management Test Cases.xlsx
+++ b/Common Documents/Test Cases/Account management Test Cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/37e01625e4e8643d/Desktop/Capgemini/Bootcamp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/37e01625e4e8643d/Documents/GitHub/PecuniaFinance/Common Documents/Test Cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_77A55CF67BECA9A8AEABF6F2BF5F2B6BAC025836" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{01508FDC-FF4A-4A0B-A3E3-9D99D2657FE2}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="11_77A55CF67BECA9A8AEABF6F2BF5F2B6BAC025836" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{111307B1-DDBB-4A38-AAAF-F6445087EE86}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="68">
   <si>
     <t>Non-Functional</t>
   </si>
@@ -150,9 +150,6 @@
     <t>&lt;blank&gt;</t>
   </si>
   <si>
-    <t>Error message:"Account Id should be of 12 digits"</t>
-  </si>
-  <si>
     <t>Error message:"Account ID should not contain alphanumeric chararcters"</t>
   </si>
   <si>
@@ -192,9 +189,6 @@
     <t>Add-Account</t>
   </si>
   <si>
-    <t>Account Id should be of 12 digits.</t>
-  </si>
-  <si>
     <t>Account Id should not have alphanumeric values</t>
   </si>
   <si>
@@ -276,19 +270,16 @@
     <t>TC_16</t>
   </si>
   <si>
-    <t>Adhaar number should be of 12 digits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                               &lt;blank&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                &lt;blank&gt;</t>
-  </si>
-  <si>
     <t>Contact number should be of 10 digits and should start with 6/7/8/9</t>
   </si>
   <si>
     <t>TC_09</t>
+  </si>
+  <si>
+    <t>Error message:"Account Id should be of 8 digits"</t>
+  </si>
+  <si>
+    <t>Account number should be of 8 digits</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1065,7 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1167,7 +1158,7 @@
         <v>3</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I4" s="31"/>
       <c r="J4" s="12"/>
@@ -1177,10 +1168,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E5" s="24" t="s">
         <v>22</v>
@@ -1189,7 +1180,7 @@
         <v>23</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H5" s="28"/>
       <c r="I5" s="20"/>
@@ -1202,10 +1193,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="E6" s="24" t="s">
         <v>22</v>
@@ -1214,7 +1205,7 @@
         <v>123</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="H6" s="28"/>
       <c r="I6" s="20"/>
@@ -1227,19 +1218,19 @@
         <v>20</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E7" s="24" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H7" s="28"/>
       <c r="I7" s="20"/>
@@ -1252,19 +1243,19 @@
         <v>21</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="24" t="s">
         <v>41</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>43</v>
       </c>
       <c r="F8" s="30">
         <v>876</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H8" s="28"/>
       <c r="I8" s="20"/>
@@ -1274,22 +1265,22 @@
     </row>
     <row r="9" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="G9" s="22" t="s">
         <v>46</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>48</v>
       </c>
       <c r="H9" s="28"/>
       <c r="I9" s="20"/>
@@ -1299,22 +1290,22 @@
     </row>
     <row r="10" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F10" s="24">
         <v>1234086</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H10" s="28"/>
       <c r="I10" s="20"/>
@@ -1324,22 +1315,22 @@
     </row>
     <row r="11" spans="1:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F11" s="30">
         <v>456</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H11" s="28"/>
       <c r="I11" s="20"/>
@@ -1349,22 +1340,22 @@
     </row>
     <row r="12" spans="1:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F12" s="30">
         <v>9876543210</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H12" s="28"/>
       <c r="I12" s="20"/>
@@ -1374,22 +1365,22 @@
     </row>
     <row r="13" spans="1:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="22" t="s">
         <v>57</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="22" t="s">
-        <v>59</v>
       </c>
       <c r="H13" s="28"/>
       <c r="I13" s="20"/>
@@ -1399,22 +1390,22 @@
     </row>
     <row r="14" spans="1:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F14" s="24" t="s">
         <v>23</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H14" s="28"/>
       <c r="I14" s="20"/>
@@ -1424,22 +1415,22 @@
     </row>
     <row r="15" spans="1:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F15" s="30">
         <v>456</v>
       </c>
       <c r="G15" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H15" s="28"/>
       <c r="I15" s="20"/>
@@ -1449,22 +1440,22 @@
     </row>
     <row r="16" spans="1:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F16" s="24" t="s">
         <v>23</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H16" s="28"/>
       <c r="I16" s="20"/>
@@ -1474,22 +1465,22 @@
     </row>
     <row r="17" spans="2:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E17" s="24" t="s">
         <v>22</v>
       </c>
       <c r="F17" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H17" s="28"/>
       <c r="I17" s="20"/>
@@ -1499,22 +1490,22 @@
     </row>
     <row r="18" spans="2:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F18" s="30">
         <v>678</v>
       </c>
       <c r="G18" s="22" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="H18" s="28"/>
       <c r="I18" s="20"/>
@@ -1524,13 +1515,13 @@
     </row>
     <row r="19" spans="2:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="E19" s="24" t="s">
         <v>22</v>
@@ -1539,7 +1530,7 @@
         <v>112233445566</v>
       </c>
       <c r="G19" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H19" s="28"/>
       <c r="I19" s="20"/>
@@ -1549,13 +1540,13 @@
     </row>
     <row r="20" spans="2:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E20" s="24" t="s">
         <v>22</v>
@@ -1564,7 +1555,7 @@
         <v>765433456767</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H20" s="28"/>
       <c r="I20" s="27"/>

</xml_diff>